<commit_message>
Fixed int to T.
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -528,7 +528,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,8 +585,8 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>

</xml_diff>